<commit_message>
new matrix per family created
</commit_message>
<xml_diff>
--- a/data/base_scenario/archetypes/pop_archetypes_citizen.xlsx
+++ b/data/base_scenario/archetypes/pop_archetypes_citizen.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\data\Kanaleneiland\archetypes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\data\base_scenario\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB87F7D2-87AB-4E7A-9E3D-EF14497534F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53CC918A-6DD9-4BD2-A390-A10F1A355783}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>name</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>WoS_type_max</t>
+  </si>
+  <si>
+    <t>WoS_time_mu</t>
+  </si>
+  <si>
+    <t>WoS_time_sigma</t>
   </si>
 </sst>
 </file>
@@ -472,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AD14"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,25 +491,25 @@
     <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="14.44140625" customWidth="1"/>
-    <col min="9" max="9" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="12" width="9.33203125" customWidth="1"/>
-    <col min="13" max="13" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="11.33203125" customWidth="1"/>
-    <col min="19" max="19" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.88671875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="18.6640625" customWidth="1"/>
-    <col min="27" max="27" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="10" width="14.44140625" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="14" width="9.33203125" customWidth="1"/>
+    <col min="15" max="15" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="11.33203125" customWidth="1"/>
+    <col min="21" max="21" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.21875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="18.6640625" customWidth="1"/>
+    <col min="29" max="29" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="23.109375" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,73 +535,79 @@
         <v>36</v>
       </c>
       <c r="I1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
         <v>37</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>39</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>40</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>16</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>17</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>19</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>25</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>26</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>27</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>28</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>29</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>30</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>31</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>32</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AE1" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AF1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -621,73 +633,79 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="J2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K2">
         <v>0</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
         <v>20</v>
       </c>
-      <c r="N2">
+      <c r="P2">
         <v>5</v>
       </c>
-      <c r="O2">
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <v>1</v>
-      </c>
       <c r="Q2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2">
         <v>1</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2">
         <v>1</v>
       </c>
       <c r="U2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V2">
+        <v>1</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
         <v>99</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>60</v>
       </c>
-      <c r="X2">
+      <c r="Z2">
         <v>15</v>
       </c>
-      <c r="Y2">
+      <c r="AA2">
         <v>15</v>
       </c>
-      <c r="Z2">
+      <c r="AB2">
         <v>340</v>
       </c>
-      <c r="AA2">
-        <v>1</v>
-      </c>
-      <c r="AB2">
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
         <v>1.5</v>
       </c>
-      <c r="AC2">
-        <v>0</v>
-      </c>
-      <c r="AD2">
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -713,73 +731,79 @@
         <v>1</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
       <c r="L3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
         <v>20</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>5</v>
       </c>
-      <c r="O3">
-        <v>1</v>
-      </c>
-      <c r="P3">
-        <v>1</v>
-      </c>
       <c r="Q3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3">
         <v>1</v>
       </c>
       <c r="S3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T3">
         <v>1</v>
       </c>
       <c r="U3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V3">
+        <v>1</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
         <v>99</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <v>60</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <v>15</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>15</v>
       </c>
-      <c r="Z3">
+      <c r="AB3">
         <v>340</v>
       </c>
-      <c r="AA3">
-        <v>1</v>
-      </c>
-      <c r="AB3">
+      <c r="AC3">
+        <v>1</v>
+      </c>
+      <c r="AD3">
         <v>1.5</v>
       </c>
-      <c r="AC3">
-        <v>0</v>
-      </c>
-      <c r="AD3">
+      <c r="AE3">
+        <v>0</v>
+      </c>
+      <c r="AF3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -805,73 +829,79 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>600</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
         <v>14</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>5</v>
       </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
       <c r="Q4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4">
         <v>1</v>
       </c>
       <c r="S4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T4">
         <v>1</v>
       </c>
       <c r="U4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4">
+        <v>1</v>
+      </c>
+      <c r="W4">
+        <v>0</v>
+      </c>
+      <c r="X4">
         <v>99</v>
       </c>
-      <c r="W4">
+      <c r="Y4">
         <v>60</v>
       </c>
-      <c r="X4">
+      <c r="Z4">
         <v>15</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>15</v>
       </c>
-      <c r="Z4">
+      <c r="AB4">
         <v>340</v>
       </c>
-      <c r="AA4">
-        <v>1</v>
-      </c>
-      <c r="AB4">
+      <c r="AC4">
+        <v>1</v>
+      </c>
+      <c r="AD4">
         <v>1.5</v>
       </c>
-      <c r="AC4">
-        <v>0</v>
-      </c>
-      <c r="AD4">
+      <c r="AE4">
+        <v>0</v>
+      </c>
+      <c r="AF4">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -897,73 +927,79 @@
         <v>1</v>
       </c>
       <c r="I5">
+        <v>600</v>
+      </c>
+      <c r="J5">
+        <v>100</v>
+      </c>
+      <c r="K5">
         <v>0.5</v>
       </c>
-      <c r="J5">
-        <v>1</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
       <c r="L5">
         <v>1</v>
       </c>
       <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
         <v>10</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>5</v>
       </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
       <c r="Q5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5">
         <v>1</v>
       </c>
       <c r="S5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T5">
         <v>1</v>
       </c>
       <c r="U5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5">
+        <v>1</v>
+      </c>
+      <c r="W5">
+        <v>0</v>
+      </c>
+      <c r="X5">
         <v>99</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>60</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
         <v>15</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>15</v>
       </c>
-      <c r="Z5">
+      <c r="AB5">
         <v>340</v>
       </c>
-      <c r="AA5">
-        <v>1</v>
-      </c>
-      <c r="AB5">
+      <c r="AC5">
+        <v>1</v>
+      </c>
+      <c r="AD5">
         <v>1.5</v>
       </c>
-      <c r="AC5">
-        <v>0</v>
-      </c>
-      <c r="AD5">
+      <c r="AE5">
+        <v>0</v>
+      </c>
+      <c r="AF5">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -989,75 +1025,79 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>600</v>
       </c>
       <c r="J6">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K6">
         <v>0</v>
       </c>
       <c r="L6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M6">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
         <v>23</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>5</v>
       </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6">
-        <v>1</v>
-      </c>
       <c r="Q6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6">
         <v>1</v>
       </c>
       <c r="S6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T6">
         <v>1</v>
       </c>
       <c r="U6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6">
+        <v>1</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
         <v>99</v>
       </c>
-      <c r="W6">
+      <c r="Y6">
         <v>60</v>
       </c>
-      <c r="X6">
+      <c r="Z6">
         <v>15</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>15</v>
       </c>
-      <c r="Z6">
+      <c r="AB6">
         <v>340</v>
       </c>
-      <c r="AA6">
-        <v>1</v>
-      </c>
-      <c r="AB6">
+      <c r="AC6">
+        <v>1</v>
+      </c>
+      <c r="AD6">
         <v>1.5</v>
       </c>
-      <c r="AC6">
-        <v>0</v>
-      </c>
-      <c r="AD6">
+      <c r="AE6">
+        <v>0</v>
+      </c>
+      <c r="AF6">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
@@ -1069,10 +1109,10 @@
       <c r="X11" s="1"/>
       <c r="Y11" s="1"/>
       <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+      <c r="AB11" s="1"/>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="P12" s="1"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
@@ -1084,10 +1124,10 @@
       <c r="X12" s="1"/>
       <c r="Y12" s="1"/>
       <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -1099,10 +1139,10 @@
       <c r="X13" s="1"/>
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AB13" s="1"/>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
@@ -1114,6 +1154,8 @@
       <c r="X14" s="1"/>
       <c r="Y14" s="1"/>
       <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AB14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
home and WoS relationship based on distance
</commit_message>
<xml_diff>
--- a/data/base_scenario/archetypes/pop_archetypes_citizen.xlsx
+++ b/data/base_scenario/archetypes/pop_archetypes_citizen.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asier.divasson\Documents\GitHub\CogniCity\data\base_scenario\archetypes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8DDE48D-1D16-48B9-B428-68F4240D318F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9EC5C21-B274-4173-8C09-BA89CF92A3A4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>name</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>walk_speed_min</t>
+  </si>
+  <si>
+    <t>dist_wos_mu</t>
+  </si>
+  <si>
+    <t>dist_wos_sigma</t>
+  </si>
+  <si>
+    <t>dist_poi_mu</t>
+  </si>
+  <si>
+    <t>dist_poi_sigma</t>
   </si>
 </sst>
 </file>
@@ -466,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AB14"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="W1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y1:AB1048576"/>
+      <selection activeCell="AB22" sqref="AB22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -497,9 +509,13 @@
     <col min="26" max="26" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="15" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -584,8 +600,20 @@
       <c r="AB1" t="s">
         <v>38</v>
       </c>
+      <c r="AC1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -670,8 +698,20 @@
       <c r="AB2">
         <v>7.4999999999999997E-2</v>
       </c>
+      <c r="AC2">
+        <v>14000</v>
+      </c>
+      <c r="AD2">
+        <v>500</v>
+      </c>
+      <c r="AE2">
+        <v>2000</v>
+      </c>
+      <c r="AF2">
+        <v>500</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -756,8 +796,20 @@
       <c r="AB3">
         <v>7.1999999999999995E-2</v>
       </c>
+      <c r="AC3">
+        <v>14000</v>
+      </c>
+      <c r="AD3">
+        <v>500</v>
+      </c>
+      <c r="AE3">
+        <v>2000</v>
+      </c>
+      <c r="AF3">
+        <v>500</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -842,8 +894,20 @@
       <c r="AB4">
         <v>4.2000000000000003E-2</v>
       </c>
+      <c r="AC4">
+        <v>2000</v>
+      </c>
+      <c r="AD4">
+        <v>500</v>
+      </c>
+      <c r="AE4">
+        <v>2000</v>
+      </c>
+      <c r="AF4">
+        <v>500</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -928,8 +992,20 @@
       <c r="AB5">
         <v>6.7000000000000004E-2</v>
       </c>
+      <c r="AC5">
+        <v>2000</v>
+      </c>
+      <c r="AD5">
+        <v>500</v>
+      </c>
+      <c r="AE5">
+        <v>2000</v>
+      </c>
+      <c r="AF5">
+        <v>500</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1014,8 +1090,20 @@
       <c r="AB6">
         <v>4.2000000000000003E-2</v>
       </c>
+      <c r="AC6">
+        <v>14000</v>
+      </c>
+      <c r="AD6">
+        <v>500</v>
+      </c>
+      <c r="AE6">
+        <v>2000</v>
+      </c>
+      <c r="AF6">
+        <v>500</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1025,7 +1113,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1035,7 +1123,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1045,7 +1133,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>

</xml_diff>